<commit_message>
simulation, resource cost working
</commit_message>
<xml_diff>
--- a/RelevantResults/ExperimentResourcevsActivity/ComparisonKValues(1_24).xlsx
+++ b/RelevantResults/ExperimentResourcevsActivity/ComparisonKValues(1_24).xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HD/Users/CamiloMontenegro/Documents/SIMOD/Github/Simod/RelevantResults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HD/Users/CamiloMontenegro/Documents/SIMOD/Github/Simod/RelevantResults/ExperimentResourcevsActivity/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>K</t>
   </si>
@@ -58,15 +58,34 @@
   <si>
     <t>Max</t>
   </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Dif_min</t>
+  </si>
+  <si>
+    <t>Dif_max</t>
+  </si>
+  <si>
+    <t>Dif_avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,20 +123,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -739,11 +761,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="2120281008"/>
-        <c:axId val="-2065379888"/>
+        <c:axId val="-2140696272"/>
+        <c:axId val="-2139694992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2120281008"/>
+        <c:axId val="-2140696272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +869,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065379888"/>
+        <c:crossAx val="-2139694992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -855,7 +877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065379888"/>
+        <c:axId val="-2139694992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8000.0"/>
@@ -963,7 +985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120281008"/>
+        <c:crossAx val="-2140696272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1622,11 +1644,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="-2074802672"/>
-        <c:axId val="-2057932672"/>
+        <c:axId val="-2139443184"/>
+        <c:axId val="-2139437088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074802672"/>
+        <c:axId val="-2139443184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,7 +1752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057932672"/>
+        <c:crossAx val="-2139437088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1738,7 +1760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2057932672"/>
+        <c:axId val="-2139437088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.02E6"/>
@@ -1846,7 +1868,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074802672"/>
+        <c:crossAx val="-2139443184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2449,11 +2471,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="-2072029024"/>
-        <c:axId val="-2077057920"/>
+        <c:axId val="-2139388912"/>
+        <c:axId val="-2139382816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072029024"/>
+        <c:axId val="-2139388912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2557,7 +2579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077057920"/>
+        <c:crossAx val="-2139382816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2565,7 +2587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077057920"/>
+        <c:axId val="-2139382816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.2E7"/>
@@ -2674,7 +2696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072029024"/>
+        <c:crossAx val="-2139388912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3086,11 +3108,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="55"/>
-        <c:axId val="-2036793184"/>
-        <c:axId val="-2037250976"/>
+        <c:axId val="-2139345632"/>
+        <c:axId val="-2139339952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2036793184"/>
+        <c:axId val="-2139345632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3194,7 +3216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2037250976"/>
+        <c:crossAx val="-2139339952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3202,7 +3224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2037250976"/>
+        <c:axId val="-2139339952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7800.0"/>
@@ -3310,7 +3332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2036793184"/>
+        <c:crossAx val="-2139345632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3722,11 +3744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="55"/>
-        <c:axId val="-2016919568"/>
-        <c:axId val="-2018057376"/>
+        <c:axId val="-2139305328"/>
+        <c:axId val="-2139300544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2016919568"/>
+        <c:axId val="-2139305328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3830,7 +3852,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2018057376"/>
+        <c:crossAx val="-2139300544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3838,7 +3860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018057376"/>
+        <c:axId val="-2139300544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.02E6"/>
@@ -3947,7 +3969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2016919568"/>
+        <c:crossAx val="-2139305328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4361,11 +4383,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="55"/>
-        <c:axId val="-2074687104"/>
-        <c:axId val="-2020301216"/>
+        <c:axId val="-2139263232"/>
+        <c:axId val="-2139257200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074687104"/>
+        <c:axId val="-2139263232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4469,7 +4491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020301216"/>
+        <c:crossAx val="-2139257200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4477,7 +4499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020301216"/>
+        <c:axId val="-2139257200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.2E7"/>
@@ -4586,7 +4608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074687104"/>
+        <c:crossAx val="-2139263232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8357,10 +8379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L53"/>
+  <dimension ref="B2:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:H16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8405,1120 +8427,1248 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>7301.1711294707002</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>919892.94889753603</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>19993722.83374</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <v>0.1</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>7480.2551329891703</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>10602.907477451299</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>377852.762654285</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>7394.4731767433996</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1011193.94672494</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>21856730.559731402</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="5"/>
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>7468.9832665722197</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>9538.7628112146995</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>356413.45261142799</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>7476.1700826876404</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>436465.63258985401</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>9175125.0557742808</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="5">
         <v>0.2</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>7207.2561312150301</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>16584.663725430401</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>492350.340399999</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>7364.4912948664996</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>412352.52708111302</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>8767503.6444485709</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="5"/>
       <c r="I6">
         <v>2</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>7275.9868768812903</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>12425.233154301501</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>411699.85101714201</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>7780.8292695084801</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>216418.15811393701</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>4592016.6857914198</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="5">
         <v>0.3</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>7477.8681198369604</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>9900.7822214483203</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <v>358136.903882857</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+      <c r="B8" s="5"/>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>7102.2564238329796</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>159840.676199863</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>3449545.6608285699</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="5"/>
       <c r="I8">
         <v>2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>7327.8238881500201</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>14647.013374828901</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <v>460710.24396571401</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>4</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>7343.2788791827397</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>72339.100306962398</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>1627683.3712885701</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="5">
         <v>0.4</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>7212.3389571091002</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>4207.5376691320698</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>240873.170362857</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
+      <c r="B10" s="5"/>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>7366.2109441838502</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>59462.340374899301</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>1378390.68496857</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="5"/>
       <c r="I10">
         <v>2</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>7395.9083873454501</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
         <v>11390.7594069158</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="1">
         <v>391043.358931428</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>7263.4641349242702</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>8971.2961604280499</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>335036.433568571</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="5">
         <v>0.5</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>7235.3515962962801</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>36479.246003890999</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>905900.15574285598</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
+      <c r="B12" s="5"/>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>7410.9070848866504</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>32216.596140985799</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>818545.07363142795</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="5"/>
       <c r="I12">
         <v>2</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>7303.7786417817797</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>8175.4453358962901</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>320732.649725714</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>6</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>7456.90149032726</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>34625.833035506403</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>880210.41589714203</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="5">
         <v>0.6</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>7488.5006476282697</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>17337.602811126599</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <v>521099.97807714198</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
+      <c r="B14" s="5"/>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>7130.4523391102302</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>8411.4596310424095</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>329154.48316857102</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="5"/>
       <c r="I14">
         <v>2</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>7436.5963377890303</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>12618.9357931141</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <v>414976.08877428499</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>7</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>7347.6184132926401</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>14922.525752638399</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>459448.14433142799</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="5">
         <v>0.7</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>7407.7978317513298</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <v>14125.217249592501</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="1">
         <v>445231.01238285599</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
+      <c r="B16" s="5"/>
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>7568.2733113464301</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>28443.607278275002</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>746786.96170857095</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="5"/>
       <c r="I16">
         <v>2</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>7129.1601374224401</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>16178.8183445374</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <v>483112.072617142</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <v>8</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>7398.9927831641198</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>19061.524778634601</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>547088.08562285698</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="5">
         <v>0.8</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>7255.4861364531298</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>19526.251020822801</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <v>550806.493022857</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
+      <c r="B18" s="5"/>
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>7369.5296233623403</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>26419.378950353199</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>695857.62366571405</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="5"/>
       <c r="I18">
         <v>2</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>7430.3540733117097</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <v>9657.1535283684698</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <v>353099.106502857</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <v>9</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>7495.1900602305404</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>30037.162270600398</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>779697.96818285598</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="5">
         <v>0.9</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>7559.1486742304296</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>40599.719954041801</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="1">
         <v>978261.16586285701</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
+      <c r="B20" s="5"/>
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>7116.1357595772397</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>6091.5475182976297</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>273328.09377428499</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="5"/>
       <c r="I20">
         <v>2</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>7591.2651765256696</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>20618.808073635199</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="1">
         <v>581997.661048571</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="1">
+      <c r="B21" s="5">
         <v>10</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>7305.4303666258802</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>25937.977750214799</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>690737.055617142</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="5">
         <v>1</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <v>7616.1374829440501</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <v>886529.01915754098</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="3">
         <v>18679904.7761028</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
+      <c r="B22" s="5"/>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>7355.5617040095403</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>13545.528784865501</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>428398.79090285703</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="5"/>
       <c r="I22">
         <v>2</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
         <v>7188.4933059082396</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>820683.13703458698</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="1">
         <v>17851155.888045698</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <v>11</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>7198.5514711637397</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>3296.4626510589401</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>216880.148882857</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
+      <c r="B24" s="5"/>
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>7262.43742279055</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>19202.545990892399</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>546384.39194285695</v>
       </c>
-      <c r="I24" t="s">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="5">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7538.3242229975103</v>
+      </c>
+      <c r="E25" s="1">
+        <v>21096.592157217499</v>
+      </c>
+      <c r="F25" s="1">
+        <v>588352.06696571305</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7396.47428851122</v>
+      </c>
+      <c r="E26" s="1">
+        <v>9831.7526632086701</v>
+      </c>
+      <c r="F26" s="1">
+        <v>353437.34322285699</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="5">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7307.2818050261203</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13838.8219727167</v>
+      </c>
+      <c r="F27" s="1">
+        <v>437681.89266000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7483.3169447151804</v>
+      </c>
+      <c r="E28" s="1">
+        <v>31403.040513161901</v>
+      </c>
+      <c r="F28" s="1">
+        <v>801610.18685142801</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="5">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>7272.60334837341</v>
+      </c>
+      <c r="E29" s="1">
+        <v>22983.527509435102</v>
+      </c>
+      <c r="F29" s="1">
+        <v>629380.16493714298</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>7617.4925544216603</v>
+      </c>
+      <c r="E30" s="1">
+        <v>8689.3025180966997</v>
+      </c>
+      <c r="F30" s="1">
+        <v>335104.77170285699</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="5">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>7673.0079273262299</v>
+      </c>
+      <c r="E31" s="1">
+        <v>13570.342705339999</v>
+      </c>
+      <c r="F31" s="1">
+        <v>431939.63504857098</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7393.50586662363</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5926.0955514032203</v>
+      </c>
+      <c r="F32" s="1">
+        <v>276253.28600857098</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="5">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7477.7458740802704</v>
+      </c>
+      <c r="E33" s="1">
+        <v>23901.9745756638</v>
+      </c>
+      <c r="F33" s="1">
+        <v>650244.45428857103</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="5"/>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>7442.9954765167304</v>
+      </c>
+      <c r="E34" s="1">
+        <v>12000.5147479193</v>
+      </c>
+      <c r="F34" s="1">
+        <v>401931.16444285703</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="5">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>7247.0466372643496</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3487.2296775120899</v>
+      </c>
+      <c r="F35" s="1">
+        <v>219651.040054285</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="5"/>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>7488.4615069557403</v>
+      </c>
+      <c r="E36" s="1">
+        <v>28255.191460973801</v>
+      </c>
+      <c r="F36" s="1">
+        <v>747679.17040571396</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="5">
+        <v>18</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>7362.4078789883497</v>
+      </c>
+      <c r="E37" s="1">
+        <v>4574.7305290791801</v>
+      </c>
+      <c r="F37" s="1">
+        <v>244551.51670571399</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="5"/>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>7450.84983055678</v>
+      </c>
+      <c r="E38" s="1">
+        <v>19427.6246164636</v>
+      </c>
+      <c r="F38" s="1">
+        <v>553292.813405714</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="5">
+        <v>19</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>7363.3810900478302</v>
+      </c>
+      <c r="E39" s="1">
+        <v>13492.1098940062</v>
+      </c>
+      <c r="F39" s="1">
+        <v>431072.53823714203</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="5"/>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7351.3683865264402</v>
+      </c>
+      <c r="E40" s="1">
+        <v>14354.334586044401</v>
+      </c>
+      <c r="F40" s="1">
+        <v>455267.79654571402</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="5">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>7301.23245251965</v>
+      </c>
+      <c r="E41" s="1">
+        <v>13370.642966416999</v>
+      </c>
+      <c r="F41" s="1">
+        <v>426350.79357428499</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="5"/>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>7209.9897479266401</v>
+      </c>
+      <c r="E42" s="1">
+        <v>10757.874770295801</v>
+      </c>
+      <c r="F42" s="1">
+        <v>371401.35494857101</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="5">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>7313.0940967036004</v>
+      </c>
+      <c r="E43" s="1">
+        <v>14194.5451091664</v>
+      </c>
+      <c r="F43" s="1">
+        <v>442975.093614285</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="5"/>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>7448.6833901292403</v>
+      </c>
+      <c r="E44" s="1">
+        <v>22752.813374653499</v>
+      </c>
+      <c r="F44" s="1">
+        <v>624702.67315428494</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="5">
+        <v>22</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
+        <v>7519.7047826320404</v>
+      </c>
+      <c r="E45" s="1">
+        <v>10814.877884461601</v>
+      </c>
+      <c r="F45" s="1">
+        <v>379576.67472285702</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" s="5"/>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>7544.9308233689699</v>
+      </c>
+      <c r="E46" s="1">
+        <v>20768.359770127099</v>
+      </c>
+      <c r="F46" s="1">
+        <v>581635.36597142799</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="5">
+        <v>23</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>7271.3978553087099</v>
+      </c>
+      <c r="E47" s="1">
+        <v>10153.769873357</v>
+      </c>
+      <c r="F47" s="1">
+        <v>360443.193237142</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="5"/>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>7552.0876932986102</v>
+      </c>
+      <c r="E48" s="1">
+        <v>9293.5185506246307</v>
+      </c>
+      <c r="F48" s="1">
+        <v>344068.04494857101</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B49" s="5">
+        <v>24</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <v>7429.5409938411603</v>
+      </c>
+      <c r="E49" s="1">
+        <v>14813.4338220877</v>
+      </c>
+      <c r="F49" s="1">
+        <v>460125.85203142802</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" s="5"/>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>7251.4256362738597</v>
+      </c>
+      <c r="E50" s="1">
+        <v>21048.952605833299</v>
+      </c>
+      <c r="F50" s="1">
+        <v>591733.02574857103</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="2">
+      <c r="D52" s="1">
+        <f>MIN(D3:D50)</f>
+        <v>7102.2564238329796</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" ref="E52:F52" si="0">MIN(E3:E50)</f>
+        <v>3296.4626510589401</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="0"/>
+        <v>216880.148882857</v>
+      </c>
+      <c r="I52" t="s">
+        <v>9</v>
+      </c>
+      <c r="J52" s="1">
         <f>MIN(J3:J22)</f>
         <v>7129.1601374224401</v>
       </c>
-      <c r="K24" s="2">
-        <f t="shared" ref="K24:L24" si="0">MIN(K3:K22)</f>
+      <c r="K52" s="1">
+        <f>MIN(K3:K22)</f>
         <v>4207.5376691320698</v>
       </c>
-      <c r="L24" s="2">
-        <f t="shared" si="0"/>
+      <c r="L52" s="1">
+        <f>MIN(L3:L22)</f>
         <v>240873.170362857</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>12</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2">
-        <v>7538.3242229975103</v>
-      </c>
-      <c r="E25" s="2">
-        <v>21096.592157217499</v>
-      </c>
-      <c r="F25" s="2">
-        <v>588352.06696571305</v>
-      </c>
-      <c r="I25" t="s">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
         <v>10</v>
       </c>
-      <c r="J25" s="2">
+      <c r="D53" s="1">
+        <f>MAX(D3:D50)</f>
+        <v>7780.8292695084801</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" ref="E53:F53" si="1">MAX(E3:E50)</f>
+        <v>1011193.94672494</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="1"/>
+        <v>21856730.559731402</v>
+      </c>
+      <c r="I53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J53" s="1">
         <f>MAX(J3:J22)</f>
         <v>7616.1374829440501</v>
       </c>
-      <c r="K25" s="2">
-        <f t="shared" ref="K25:L25" si="1">MAX(K3:K22)</f>
+      <c r="K53" s="1">
+        <f>MAX(K3:K22)</f>
         <v>886529.01915754098</v>
       </c>
-      <c r="L25" s="2">
-        <f t="shared" si="1"/>
+      <c r="L53" s="1">
+        <f>MAX(L3:L22)</f>
         <v>18679904.7761028</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2">
-        <v>7396.47428851122</v>
-      </c>
-      <c r="E26" s="2">
-        <v>9831.7526632086701</v>
-      </c>
-      <c r="F26" s="2">
-        <v>353437.34322285699</v>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="1">
+        <f>AVERAGE(D3:D50)</f>
+        <v>7385.7641307546155</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" ref="E54:F54" si="2">AVERAGE(E3:E50)</f>
+        <v>82373.973987253426</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="2"/>
+        <v>1890181.9600188078</v>
+      </c>
+      <c r="I54" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" s="1">
+        <f>AVERAGE(J3:J22)</f>
+        <v>7374.4245401070802</v>
+      </c>
+      <c r="K54" s="1">
+        <f>AVERAGE(K3:K22)</f>
+        <v>99591.350707393867</v>
+      </c>
+      <c r="L54" s="1">
+        <f>AVERAGE(L3:L22)</f>
+        <v>2258767.8565865671</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="4">
+        <f>(D52-J52)/D52</f>
+        <v>-3.788051568960526E-3</v>
+      </c>
+      <c r="E56" s="4">
+        <f t="shared" ref="E56:F56" si="3">(E52-K52)/E52</f>
+        <v>-0.27637959671117773</v>
+      </c>
+      <c r="F56" s="4">
+        <f t="shared" si="3"/>
+        <v>-0.11062802014655243</v>
+      </c>
+      <c r="I56" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" s="4">
+        <f>(J52-D52)/J52</f>
+        <v>3.7737563851648276E-3</v>
+      </c>
+      <c r="K56" s="4">
+        <f t="shared" ref="K56:L56" si="4">(K52-E52)/K52</f>
+        <v>0.21653401341052431</v>
+      </c>
+      <c r="L56" s="4">
+        <f t="shared" si="4"/>
+        <v>9.9608526112959547E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
         <v>13</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2">
-        <v>7307.2818050261203</v>
-      </c>
-      <c r="E27" s="2">
-        <v>13838.8219727167</v>
-      </c>
-      <c r="F27" s="2">
-        <v>437681.89266000001</v>
+      <c r="D57" s="4">
+        <f>(D53-J53)/D53</f>
+        <v>2.1166353978466577E-2</v>
+      </c>
+      <c r="E57" s="4">
+        <f t="shared" ref="E57:F57" si="5">(E53-K53)/E53</f>
+        <v>0.12328488315338949</v>
+      </c>
+      <c r="F57" s="4">
+        <f t="shared" si="5"/>
+        <v>0.14534771222744311</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="4">
+        <f t="shared" ref="J57:J58" si="6">(J53-D53)/J53</f>
+        <v>-2.1624056410910232E-2</v>
+      </c>
+      <c r="K57" s="4">
+        <f t="shared" ref="K57:K58" si="7">(K53-E53)/K53</f>
+        <v>-0.14062137264933158</v>
+      </c>
+      <c r="L57" s="4">
+        <f t="shared" ref="L57:L58" si="8">(L53-F53)/L53</f>
+        <v>-0.17006648704616067</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="1"/>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2">
-        <v>7483.3169447151804</v>
-      </c>
-      <c r="E28" s="2">
-        <v>31403.040513161901</v>
-      </c>
-      <c r="F28" s="2">
-        <v>801610.18685142801</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
         <v>14</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
-        <v>7272.60334837341</v>
-      </c>
-      <c r="E29" s="2">
-        <v>22983.527509435102</v>
-      </c>
-      <c r="F29" s="2">
-        <v>629380.16493714298</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2">
-        <v>7617.4925544216603</v>
-      </c>
-      <c r="E30" s="2">
-        <v>8689.3025180966997</v>
-      </c>
-      <c r="F30" s="2">
-        <v>335104.77170285699</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>15</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
-        <v>7673.0079273262299</v>
-      </c>
-      <c r="E31" s="2">
-        <v>13570.342705339999</v>
-      </c>
-      <c r="F31" s="2">
-        <v>431939.63504857098</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2">
-        <v>7393.50586662363</v>
-      </c>
-      <c r="E32" s="2">
-        <v>5926.0955514032203</v>
-      </c>
-      <c r="F32" s="2">
-        <v>276253.28600857098</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="1">
-        <v>16</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
-        <v>7477.7458740802704</v>
-      </c>
-      <c r="E33" s="2">
-        <v>23901.9745756638</v>
-      </c>
-      <c r="F33" s="2">
-        <v>650244.45428857103</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2">
-        <v>7442.9954765167304</v>
-      </c>
-      <c r="E34" s="2">
-        <v>12000.5147479193</v>
-      </c>
-      <c r="F34" s="2">
-        <v>401931.16444285703</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="1">
-        <v>17</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2">
-        <v>7247.0466372643496</v>
-      </c>
-      <c r="E35" s="2">
-        <v>3487.2296775120899</v>
-      </c>
-      <c r="F35" s="2">
-        <v>219651.040054285</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2">
-        <v>7488.4615069557403</v>
-      </c>
-      <c r="E36" s="2">
-        <v>28255.191460973801</v>
-      </c>
-      <c r="F36" s="2">
-        <v>747679.17040571396</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="1">
-        <v>18</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2">
-        <v>7362.4078789883497</v>
-      </c>
-      <c r="E37" s="2">
-        <v>4574.7305290791801</v>
-      </c>
-      <c r="F37" s="2">
-        <v>244551.51670571399</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2">
-        <v>7450.84983055678</v>
-      </c>
-      <c r="E38" s="2">
-        <v>19427.6246164636</v>
-      </c>
-      <c r="F38" s="2">
-        <v>553292.813405714</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="1">
-        <v>19</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2">
-        <v>7363.3810900478302</v>
-      </c>
-      <c r="E39" s="2">
-        <v>13492.1098940062</v>
-      </c>
-      <c r="F39" s="2">
-        <v>431072.53823714203</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" s="2">
-        <v>7351.3683865264402</v>
-      </c>
-      <c r="E40" s="2">
-        <v>14354.334586044401</v>
-      </c>
-      <c r="F40" s="2">
-        <v>455267.79654571402</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="1">
-        <v>20</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2">
-        <v>7301.23245251965</v>
-      </c>
-      <c r="E41" s="2">
-        <v>13370.642966416999</v>
-      </c>
-      <c r="F41" s="2">
-        <v>426350.79357428499</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" s="2">
-        <v>7209.9897479266401</v>
-      </c>
-      <c r="E42" s="2">
-        <v>10757.874770295801</v>
-      </c>
-      <c r="F42" s="2">
-        <v>371401.35494857101</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="1">
-        <v>21</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2">
-        <v>7313.0940967036004</v>
-      </c>
-      <c r="E43" s="2">
-        <v>14194.5451091664</v>
-      </c>
-      <c r="F43" s="2">
-        <v>442975.093614285</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44" s="2">
-        <v>7448.6833901292403</v>
-      </c>
-      <c r="E44" s="2">
-        <v>22752.813374653499</v>
-      </c>
-      <c r="F44" s="2">
-        <v>624702.67315428494</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="1">
-        <v>22</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2">
-        <v>7519.7047826320404</v>
-      </c>
-      <c r="E45" s="2">
-        <v>10814.877884461601</v>
-      </c>
-      <c r="F45" s="2">
-        <v>379576.67472285702</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" s="2">
-        <v>7544.9308233689699</v>
-      </c>
-      <c r="E46" s="2">
-        <v>20768.359770127099</v>
-      </c>
-      <c r="F46" s="2">
-        <v>581635.36597142799</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="1">
-        <v>23</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2">
-        <v>7271.3978553087099</v>
-      </c>
-      <c r="E47" s="2">
-        <v>10153.769873357</v>
-      </c>
-      <c r="F47" s="2">
-        <v>360443.193237142</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" s="2">
-        <v>7552.0876932986102</v>
-      </c>
-      <c r="E48" s="2">
-        <v>9293.5185506246307</v>
-      </c>
-      <c r="F48" s="2">
-        <v>344068.04494857101</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="1">
-        <v>24</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2">
-        <v>7429.5409938411603</v>
-      </c>
-      <c r="E49" s="2">
-        <v>14813.4338220877</v>
-      </c>
-      <c r="F49" s="2">
-        <v>460125.85203142802</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50" s="2">
-        <v>7251.4256362738597</v>
-      </c>
-      <c r="E50" s="2">
-        <v>21048.952605833299</v>
-      </c>
-      <c r="F50" s="2">
-        <v>591733.02574857103</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="2">
-        <f>MIN(D3:D50)</f>
-        <v>7102.2564238329796</v>
-      </c>
-      <c r="E52" s="2">
-        <f t="shared" ref="E52:F52" si="2">MIN(E3:E50)</f>
-        <v>3296.4626510589401</v>
-      </c>
-      <c r="F52" s="2">
-        <f t="shared" si="2"/>
-        <v>216880.148882857</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="2">
-        <f>MAX(D3:D50)</f>
-        <v>7780.8292695084801</v>
-      </c>
-      <c r="E53" s="2">
-        <f t="shared" ref="E53:F53" si="3">MAX(E3:E50)</f>
-        <v>1011193.94672494</v>
-      </c>
-      <c r="F53" s="2">
-        <f t="shared" si="3"/>
-        <v>21856730.559731402</v>
+      <c r="D58" s="4">
+        <f>(D54-J54)/D54</f>
+        <v>1.5353307317677197E-3</v>
+      </c>
+      <c r="E58" s="4">
+        <f t="shared" ref="E58" si="9">(E54-K54)/E54</f>
+        <v>-0.20901476384767673</v>
+      </c>
+      <c r="F58" s="4">
+        <f t="shared" ref="F58" si="10">(F54-L54)/F54</f>
+        <v>-0.19500021921915486</v>
+      </c>
+      <c r="I58" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="4">
+        <f t="shared" si="6"/>
+        <v>-1.5376915969324712E-3</v>
+      </c>
+      <c r="K58" s="4">
+        <f t="shared" si="7"/>
+        <v>0.17288024108364852</v>
+      </c>
+      <c r="L58" s="4">
+        <f t="shared" si="8"/>
+        <v>0.16318006983009026</v>
       </c>
     </row>
   </sheetData>
@@ -9533,11 +9683,6 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="H13:H14"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B30"/>
@@ -9545,11 +9690,11 @@
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
@@ -9557,6 +9702,11 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>